<commit_message>
Added new sheets with relevant metadata
</commit_message>
<xml_diff>
--- a/MATLAB/Examples/eds_data/eds_mineral_data.xlsx
+++ b/MATLAB/Examples/eds_data/eds_mineral_data.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18596\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18596\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09487D76-0075-4339-B4E3-E41BF1121D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AD2DC4-26B7-4170-8C22-94906803C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BAD38CB1-F542-45E1-992C-A4E902F467C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BAD38CB1-F542-45E1-992C-A4E902F467C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Net_Intensity" sheetId="1" r:id="rId1"/>
     <sheet name="Atom_Percent" sheetId="2" r:id="rId2"/>
-    <sheet name="README" sheetId="3" r:id="rId3"/>
+    <sheet name="Reference_Minerals" sheetId="4" r:id="rId3"/>
+    <sheet name="Microscopy_Info" sheetId="5" r:id="rId4"/>
+    <sheet name="README" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4426" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4557" uniqueCount="138">
   <si>
     <t>Albite</t>
   </si>
@@ -233,6 +235,225 @@
   </si>
   <si>
     <t>EDS atom percent data normalized to 100%. Does not include chemical information for the elements C, N, or O.</t>
+  </si>
+  <si>
+    <t>Reference_Minerals</t>
+  </si>
+  <si>
+    <t>CATALOG_NUMBER</t>
+  </si>
+  <si>
+    <t>SPECIMEN_NAME</t>
+  </si>
+  <si>
+    <t>CONTINENT</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>LATITUDE_N</t>
+  </si>
+  <si>
+    <t>LONGITUDE_E</t>
+  </si>
+  <si>
+    <t>NMNH C5390-00</t>
+  </si>
+  <si>
+    <t>NMNH 121066-00</t>
+  </si>
+  <si>
+    <t>NMNH 122946-01</t>
+  </si>
+  <si>
+    <t>NMNH 95997-00</t>
+  </si>
+  <si>
+    <t>NMNH 135065-00</t>
+  </si>
+  <si>
+    <t>NMNH 161151-00</t>
+  </si>
+  <si>
+    <t>NMNH 106247-00</t>
+  </si>
+  <si>
+    <t>NMNH 80165-01</t>
+  </si>
+  <si>
+    <t>NMNH 120901-00</t>
+  </si>
+  <si>
+    <t>NMNH B18392-00</t>
+  </si>
+  <si>
+    <t>NMNH 126237-00</t>
+  </si>
+  <si>
+    <t>NMNH B18239-00</t>
+  </si>
+  <si>
+    <t>NMNH 144954-03</t>
+  </si>
+  <si>
+    <t>NMNH 117329-00</t>
+  </si>
+  <si>
+    <t>NMNH 95658-00</t>
+  </si>
+  <si>
+    <t>NMNH B18247-00</t>
+  </si>
+  <si>
+    <t>NMNH 174748-00</t>
+  </si>
+  <si>
+    <t>NMNH 117609-00</t>
+  </si>
+  <si>
+    <t>Muscovite (var. Illite)</t>
+  </si>
+  <si>
+    <t>Enstatite (var. bronzite)</t>
+  </si>
+  <si>
+    <t>Fluorapatite</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Virginia; Amelia Co.; Rutherford Mine</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Maryland; Howard Co.; Quarry Near Marriottsville</t>
+  </si>
+  <si>
+    <t>Illinois; 4896861</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Quebec; Huberdeau</t>
+  </si>
+  <si>
+    <t>Oregon; Lake Co.; Warner Valley, Sagebrush Flat</t>
+  </si>
+  <si>
+    <t>North Carolina; Cleveland Co.; Foote Mineral Company Spodumene Mine; Kings Mtn. (near)</t>
+  </si>
+  <si>
+    <t>California; San Diego Co.; Otay</t>
+  </si>
+  <si>
+    <t>North Carolina; Hawk Mica Mine; Bakersville (near)</t>
+  </si>
+  <si>
+    <t>Montana; Zonolite Company Mine; Libby</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Sicily; Monte Etna</t>
+  </si>
+  <si>
+    <t>Ontario; Silver Crater Mine; Wiberforce (near)</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Styria; Kraubat</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Telemark; Kragero</t>
+  </si>
+  <si>
+    <t>Utah; Garfield Co.; Kaibab Fault (W Slope of) (?); Panguitch (near)</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Heinola</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Ratnapura District; Kongastota</t>
+  </si>
+  <si>
+    <t>Ontario; Renfrew Co.; Turner Island; 6119449</t>
+  </si>
+  <si>
+    <t>Smithsonian Institution National Museum of Natural History (NMNH) mineral catalog numbers.</t>
+  </si>
+  <si>
+    <t>Titanite (aka sphene)</t>
+  </si>
+  <si>
+    <t>Electron microscopy details.</t>
+  </si>
+  <si>
+    <t>Microscopy_Info</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>SAMPLE COATING</t>
+  </si>
+  <si>
+    <t>SAMPLE PREPARATION</t>
+  </si>
+  <si>
+    <t>Mineral samples powdered with a mortar and pestle. Powders sprinkled onto aluminum SEM pin mounts with double-sided carbon adhesive tabs. Loose material blown away with air under a fume hood.</t>
+  </si>
+  <si>
+    <t>10-20 nm carbon coat | Leica EM ACE600</t>
+  </si>
+  <si>
+    <t>MICROSCOPE</t>
+  </si>
+  <si>
+    <t>Quattro Environmental Scanning Electron Microscope</t>
+  </si>
+  <si>
+    <t>EDS DETECTOR</t>
+  </si>
+  <si>
+    <t>EDAX Octane Elect Super</t>
+  </si>
+  <si>
+    <t>OPERATING CONDITIONS</t>
+  </si>
+  <si>
+    <t>15 kV acceleration voltage | 11 nA beam current | 12 mm working distance | 10 s Live Time for EDS acquistion</t>
+  </si>
+  <si>
+    <t>Center for Electron Microscopy and Analysis (CEMAS), The Ohio State University, Columbus, Ohio, USA</t>
   </si>
 </sst>
 </file>
@@ -636,7 +857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39454,7 +39675,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78280,16 +78501,584 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB2CE49-DCC6-478E-A662-DD2ECDC173ED}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921AFB84-FBDC-43CC-AF06-5661387E5E74}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2">
+        <v>37.344999999999999</v>
+      </c>
+      <c r="H2">
+        <v>-77.944999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3">
+        <v>37.75</v>
+      </c>
+      <c r="H3">
+        <v>14.983000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4">
+        <v>44.25</v>
+      </c>
+      <c r="H4">
+        <v>-79.082999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5">
+        <v>39.363999999999997</v>
+      </c>
+      <c r="H5">
+        <v>-76.899000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8">
+        <v>58.884999999999998</v>
+      </c>
+      <c r="H8">
+        <v>9.4250000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9">
+        <v>45.982999999999997</v>
+      </c>
+      <c r="H9">
+        <v>-74.632999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10">
+        <v>42.082999999999998</v>
+      </c>
+      <c r="H10">
+        <v>-119.917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11">
+        <v>35.210999999999999</v>
+      </c>
+      <c r="H11">
+        <v>-81.355999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12">
+        <v>32.633000000000003</v>
+      </c>
+      <c r="H12">
+        <v>-116.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13">
+        <v>39.75</v>
+      </c>
+      <c r="H13">
+        <v>-89.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14">
+        <v>36.017000000000003</v>
+      </c>
+      <c r="H14">
+        <v>-82.091999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15">
+        <v>37.82</v>
+      </c>
+      <c r="H15">
+        <v>-112.435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17">
+        <v>6.58</v>
+      </c>
+      <c r="H17">
+        <v>80.564999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18">
+        <v>45.695</v>
+      </c>
+      <c r="H18">
+        <v>-77.355000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19">
+        <v>48.470999999999997</v>
+      </c>
+      <c r="H19">
+        <v>-115.42100000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I19">
+    <sortCondition ref="B2:B19"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B365B494-4B18-4D13-A016-11C9050C3B92}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB2CE49-DCC6-478E-A662-DD2ECDC173ED}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -78316,6 +79105,22 @@
         <v>64</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>